<commit_message>
able to mix wafer poorly
</commit_message>
<xml_diff>
--- a/BTRAN Wafer Map 93361-01.xlsx
+++ b/BTRAN Wafer Map 93361-01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fcd1d2a289e3a233/Escritorio/Python/Ideal_Power_ideas/excel_replica-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://idealpowerinc-my.sharepoint.com/personal/leonardo_viana_idealpower_com/Documents/Desktop/excel_replica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{12A5F069-290D-4CAF-A721-DA5D196BF305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFFE004C-1547-4BE3-A1D2-B965A318CA87}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{12A5F069-290D-4CAF-A721-DA5D196BF305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C116770-3021-4697-848B-15664EA993BF}"/>
   <bookViews>
-    <workbookView xWindow="14805" yWindow="0" windowWidth="9795" windowHeight="13710" xr2:uid="{5C87E352-BAD7-4E1A-B122-0857B26F3796}"/>
+    <workbookView xWindow="7200" yWindow="45" windowWidth="21600" windowHeight="11235" xr2:uid="{5C87E352-BAD7-4E1A-B122-0857B26F3796}"/>
   </bookViews>
   <sheets>
     <sheet name="Wafer" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="119">
   <si>
     <t>BiTRAN Wafer Yield Map</t>
   </si>
@@ -412,12 +412,6 @@
   </si>
   <si>
     <t>V</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>Joe &amp; Yifan</t>
   </si>
   <si>
     <t>Avg F</t>
@@ -1082,6 +1076,52 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="180"/>
     </xf>
@@ -1097,52 +1137,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2717,7 +2711,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -3018,11 +3012,11 @@
   </sheetPr>
   <dimension ref="A1:Y140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" customWidth="1"/>
@@ -3037,13 +3031,13 @@
   <sheetData>
     <row r="1" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
@@ -3061,9 +3055,7 @@
       <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="47" t="s">
-        <v>117</v>
-      </c>
+      <c r="E2" s="47"/>
       <c r="F2" s="3"/>
       <c r="G2" s="4" t="s">
         <v>3</v>
@@ -3102,9 +3094,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
-        <v>118</v>
-      </c>
+      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="2"/>
@@ -3123,10 +3113,10 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="R5" s="73"/>
-      <c r="S5" s="73"/>
-      <c r="T5" s="73"/>
-      <c r="U5" s="73"/>
+      <c r="R5" s="61"/>
+      <c r="S5" s="61"/>
+      <c r="T5" s="61"/>
+      <c r="U5" s="61"/>
     </row>
     <row r="6" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
@@ -3152,28 +3142,28 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="2"/>
-      <c r="O6" s="74"/>
+      <c r="O6" s="62"/>
       <c r="P6" s="42"/>
-      <c r="Q6" s="60" t="s">
+      <c r="Q6" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="R6" s="60" t="s">
+      <c r="R6" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="S6" s="60" t="s">
+      <c r="S6" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="T6" s="60" t="s">
+      <c r="T6" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="U6" s="60" t="s">
+      <c r="U6" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="V6" s="60" t="s">
+      <c r="V6" s="57" t="s">
         <v>15</v>
       </c>
       <c r="W6" s="42"/>
-      <c r="X6" s="61"/>
+      <c r="X6" s="69"/>
     </row>
     <row r="7" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
@@ -3199,16 +3189,16 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="2"/>
-      <c r="O7" s="74"/>
+      <c r="O7" s="62"/>
       <c r="P7" s="42"/>
-      <c r="Q7" s="60"/>
-      <c r="R7" s="60"/>
-      <c r="S7" s="60"/>
-      <c r="T7" s="60"/>
-      <c r="U7" s="60"/>
-      <c r="V7" s="60"/>
+      <c r="Q7" s="57"/>
+      <c r="R7" s="57"/>
+      <c r="S7" s="57"/>
+      <c r="T7" s="57"/>
+      <c r="U7" s="57"/>
+      <c r="V7" s="57"/>
       <c r="W7" s="42"/>
-      <c r="X7" s="61"/>
+      <c r="X7" s="69"/>
     </row>
     <row r="8" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
@@ -3234,16 +3224,16 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="2"/>
-      <c r="O8" s="74"/>
+      <c r="O8" s="62"/>
       <c r="P8" s="42"/>
-      <c r="Q8" s="60"/>
-      <c r="R8" s="60"/>
-      <c r="S8" s="60"/>
-      <c r="T8" s="60"/>
-      <c r="U8" s="60"/>
-      <c r="V8" s="60"/>
+      <c r="Q8" s="57"/>
+      <c r="R8" s="57"/>
+      <c r="S8" s="57"/>
+      <c r="T8" s="57"/>
+      <c r="U8" s="57"/>
+      <c r="V8" s="57"/>
       <c r="W8" s="42"/>
-      <c r="X8" s="61"/>
+      <c r="X8" s="69"/>
     </row>
     <row r="9" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
@@ -3274,28 +3264,28 @@
       <c r="J9" s="5"/>
       <c r="K9" s="2"/>
       <c r="O9" s="42"/>
-      <c r="P9" s="66" t="s">
+      <c r="P9" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="Q9" s="60" t="s">
+      <c r="Q9" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="R9" s="60" t="s">
+      <c r="R9" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="S9" s="60" t="s">
+      <c r="S9" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="T9" s="60" t="s">
+      <c r="T9" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="U9" s="60" t="s">
+      <c r="U9" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="V9" s="60" t="s">
+      <c r="V9" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="W9" s="69" t="s">
+      <c r="W9" s="63" t="s">
         <v>18</v>
       </c>
       <c r="X9" s="42"/>
@@ -3329,14 +3319,14 @@
       <c r="J10" s="5"/>
       <c r="K10" s="2"/>
       <c r="O10" s="42"/>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="60"/>
-      <c r="S10" s="60"/>
-      <c r="T10" s="60"/>
-      <c r="U10" s="60"/>
-      <c r="V10" s="60"/>
-      <c r="W10" s="70"/>
+      <c r="P10" s="59"/>
+      <c r="Q10" s="57"/>
+      <c r="R10" s="57"/>
+      <c r="S10" s="57"/>
+      <c r="T10" s="57"/>
+      <c r="U10" s="57"/>
+      <c r="V10" s="57"/>
+      <c r="W10" s="64"/>
       <c r="X10" s="42"/>
     </row>
     <row r="11" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3368,14 +3358,14 @@
       <c r="J11" s="5"/>
       <c r="K11" s="2"/>
       <c r="O11" s="42"/>
-      <c r="P11" s="68"/>
-      <c r="Q11" s="60"/>
-      <c r="R11" s="60"/>
-      <c r="S11" s="60"/>
-      <c r="T11" s="60"/>
-      <c r="U11" s="60"/>
-      <c r="V11" s="60"/>
-      <c r="W11" s="71"/>
+      <c r="P11" s="60"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="57"/>
+      <c r="S11" s="57"/>
+      <c r="T11" s="57"/>
+      <c r="U11" s="57"/>
+      <c r="V11" s="57"/>
+      <c r="W11" s="65"/>
       <c r="X11" s="42"/>
     </row>
     <row r="12" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3410,34 +3400,34 @@
         <v>57.856033325200002</v>
       </c>
       <c r="K12" s="2"/>
-      <c r="O12" s="60" t="s">
+      <c r="O12" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="P12" s="60" t="s">
+      <c r="P12" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="Q12" s="60" t="s">
+      <c r="Q12" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="R12" s="60" t="s">
+      <c r="R12" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="S12" s="60" t="s">
+      <c r="S12" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="T12" s="60" t="s">
+      <c r="T12" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="U12" s="60" t="s">
+      <c r="U12" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="V12" s="60" t="s">
+      <c r="V12" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="W12" s="60" t="s">
+      <c r="W12" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="X12" s="60" t="s">
+      <c r="X12" s="57" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3473,16 +3463,16 @@
         <v>107</v>
       </c>
       <c r="K13" s="2"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="60"/>
-      <c r="S13" s="60"/>
-      <c r="T13" s="60"/>
-      <c r="U13" s="60"/>
-      <c r="V13" s="60"/>
-      <c r="W13" s="60"/>
-      <c r="X13" s="60"/>
+      <c r="O13" s="57"/>
+      <c r="P13" s="57"/>
+      <c r="Q13" s="57"/>
+      <c r="R13" s="57"/>
+      <c r="S13" s="57"/>
+      <c r="T13" s="57"/>
+      <c r="U13" s="57"/>
+      <c r="V13" s="57"/>
+      <c r="W13" s="57"/>
+      <c r="X13" s="57"/>
     </row>
     <row r="14" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
@@ -3516,16 +3506,16 @@
         <v>54.325862884499998</v>
       </c>
       <c r="K14" s="2"/>
-      <c r="O14" s="60"/>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="60"/>
-      <c r="R14" s="60"/>
-      <c r="S14" s="60"/>
-      <c r="T14" s="60"/>
-      <c r="U14" s="60"/>
-      <c r="V14" s="60"/>
-      <c r="W14" s="60"/>
-      <c r="X14" s="60"/>
+      <c r="O14" s="57"/>
+      <c r="P14" s="57"/>
+      <c r="Q14" s="57"/>
+      <c r="R14" s="57"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="57"/>
+      <c r="U14" s="57"/>
+      <c r="V14" s="57"/>
+      <c r="W14" s="57"/>
+      <c r="X14" s="57"/>
     </row>
     <row r="15" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="43">
@@ -3558,41 +3548,41 @@
       <c r="J15" s="43">
         <v>58.232452392600003</v>
       </c>
-      <c r="K15" s="65" t="s">
+      <c r="K15" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="N15" s="62"/>
-      <c r="O15" s="60" t="s">
+      <c r="N15" s="70"/>
+      <c r="O15" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="P15" s="60" t="s">
+      <c r="P15" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="Q15" s="60" t="s">
+      <c r="Q15" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="R15" s="60" t="s">
+      <c r="R15" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="S15" s="60" t="s">
+      <c r="S15" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="T15" s="60" t="s">
+      <c r="T15" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="U15" s="60" t="s">
+      <c r="U15" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="V15" s="60" t="s">
+      <c r="V15" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="W15" s="60" t="s">
+      <c r="W15" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="X15" s="60" t="s">
+      <c r="X15" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="Y15" s="55"/>
+      <c r="Y15" s="71"/>
     </row>
     <row r="16" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
@@ -3625,19 +3615,19 @@
       <c r="J16" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="K16" s="65"/>
-      <c r="N16" s="62"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="60"/>
-      <c r="R16" s="60"/>
-      <c r="S16" s="60"/>
-      <c r="T16" s="60"/>
-      <c r="U16" s="60"/>
-      <c r="V16" s="60"/>
-      <c r="W16" s="60"/>
-      <c r="X16" s="60"/>
-      <c r="Y16" s="55"/>
+      <c r="K16" s="68"/>
+      <c r="N16" s="70"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="57"/>
+      <c r="Q16" s="57"/>
+      <c r="R16" s="57"/>
+      <c r="S16" s="57"/>
+      <c r="T16" s="57"/>
+      <c r="U16" s="57"/>
+      <c r="V16" s="57"/>
+      <c r="W16" s="57"/>
+      <c r="X16" s="57"/>
+      <c r="Y16" s="71"/>
     </row>
     <row r="17" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
@@ -3670,19 +3660,19 @@
       <c r="J17" s="8">
         <v>55.9235725403</v>
       </c>
-      <c r="K17" s="65"/>
-      <c r="N17" s="62"/>
-      <c r="O17" s="60"/>
-      <c r="P17" s="60"/>
-      <c r="Q17" s="60"/>
-      <c r="R17" s="60"/>
-      <c r="S17" s="60"/>
-      <c r="T17" s="60"/>
-      <c r="U17" s="60"/>
-      <c r="V17" s="60"/>
-      <c r="W17" s="60"/>
-      <c r="X17" s="60"/>
-      <c r="Y17" s="55"/>
+      <c r="K17" s="68"/>
+      <c r="N17" s="70"/>
+      <c r="O17" s="57"/>
+      <c r="P17" s="57"/>
+      <c r="Q17" s="57"/>
+      <c r="R17" s="57"/>
+      <c r="S17" s="57"/>
+      <c r="T17" s="57"/>
+      <c r="U17" s="57"/>
+      <c r="V17" s="57"/>
+      <c r="W17" s="57"/>
+      <c r="X17" s="57"/>
+      <c r="Y17" s="71"/>
     </row>
     <row r="18" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
@@ -3715,39 +3705,39 @@
       <c r="J18" s="6">
         <v>59.235572814900003</v>
       </c>
-      <c r="K18" s="65"/>
-      <c r="N18" s="62"/>
-      <c r="O18" s="60" t="s">
+      <c r="K18" s="68"/>
+      <c r="N18" s="70"/>
+      <c r="O18" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="P18" s="60" t="s">
+      <c r="P18" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="Q18" s="60" t="s">
+      <c r="Q18" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="R18" s="60" t="s">
+      <c r="R18" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="S18" s="60" t="s">
+      <c r="S18" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="T18" s="60" t="s">
+      <c r="T18" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="U18" s="60" t="s">
+      <c r="U18" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="V18" s="60" t="s">
+      <c r="V18" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="W18" s="60" t="s">
+      <c r="W18" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="X18" s="60" t="s">
+      <c r="X18" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="Y18" s="55"/>
+      <c r="Y18" s="71"/>
     </row>
     <row r="19" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
@@ -3780,19 +3770,19 @@
       <c r="J19" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="K19" s="65"/>
-      <c r="N19" s="62"/>
-      <c r="O19" s="60"/>
-      <c r="P19" s="60"/>
-      <c r="Q19" s="60"/>
-      <c r="R19" s="60"/>
-      <c r="S19" s="60"/>
-      <c r="T19" s="60"/>
-      <c r="U19" s="60"/>
-      <c r="V19" s="60"/>
-      <c r="W19" s="60"/>
-      <c r="X19" s="60"/>
-      <c r="Y19" s="55"/>
+      <c r="K19" s="68"/>
+      <c r="N19" s="70"/>
+      <c r="O19" s="57"/>
+      <c r="P19" s="57"/>
+      <c r="Q19" s="57"/>
+      <c r="R19" s="57"/>
+      <c r="S19" s="57"/>
+      <c r="T19" s="57"/>
+      <c r="U19" s="57"/>
+      <c r="V19" s="57"/>
+      <c r="W19" s="57"/>
+      <c r="X19" s="57"/>
+      <c r="Y19" s="71"/>
     </row>
     <row r="20" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
@@ -3825,19 +3815,19 @@
       <c r="J20" s="10">
         <v>59.560184478799997</v>
       </c>
-      <c r="K20" s="65"/>
-      <c r="N20" s="62"/>
-      <c r="O20" s="60"/>
-      <c r="P20" s="60"/>
-      <c r="Q20" s="60"/>
-      <c r="R20" s="60"/>
-      <c r="S20" s="60"/>
-      <c r="T20" s="60"/>
-      <c r="U20" s="60"/>
-      <c r="V20" s="60"/>
-      <c r="W20" s="60"/>
-      <c r="X20" s="60"/>
-      <c r="Y20" s="55"/>
+      <c r="K20" s="68"/>
+      <c r="N20" s="70"/>
+      <c r="O20" s="57"/>
+      <c r="P20" s="57"/>
+      <c r="Q20" s="57"/>
+      <c r="R20" s="57"/>
+      <c r="S20" s="57"/>
+      <c r="T20" s="57"/>
+      <c r="U20" s="57"/>
+      <c r="V20" s="57"/>
+      <c r="W20" s="57"/>
+      <c r="X20" s="57"/>
+      <c r="Y20" s="71"/>
     </row>
     <row r="21" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
@@ -3870,39 +3860,39 @@
       <c r="J21" s="6">
         <v>48.2919921875</v>
       </c>
-      <c r="K21" s="65"/>
-      <c r="N21" s="62"/>
-      <c r="O21" s="60" t="s">
+      <c r="K21" s="68"/>
+      <c r="N21" s="70"/>
+      <c r="O21" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="P21" s="60" t="s">
+      <c r="P21" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="Q21" s="60" t="s">
+      <c r="Q21" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="R21" s="60" t="s">
+      <c r="R21" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="S21" s="60" t="s">
+      <c r="S21" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="T21" s="60" t="s">
+      <c r="T21" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="U21" s="60" t="s">
+      <c r="U21" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="V21" s="60" t="s">
+      <c r="V21" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="W21" s="60" t="s">
+      <c r="W21" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="X21" s="60" t="s">
+      <c r="X21" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="Y21" s="55"/>
+      <c r="Y21" s="71"/>
     </row>
     <row r="22" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
@@ -3935,19 +3925,19 @@
       <c r="J22" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="K22" s="65"/>
-      <c r="N22" s="62"/>
-      <c r="O22" s="60"/>
-      <c r="P22" s="60"/>
-      <c r="Q22" s="60"/>
-      <c r="R22" s="60"/>
-      <c r="S22" s="60"/>
-      <c r="T22" s="60"/>
-      <c r="U22" s="60"/>
-      <c r="V22" s="60"/>
-      <c r="W22" s="60"/>
-      <c r="X22" s="60"/>
-      <c r="Y22" s="55"/>
+      <c r="K22" s="68"/>
+      <c r="N22" s="70"/>
+      <c r="O22" s="57"/>
+      <c r="P22" s="57"/>
+      <c r="Q22" s="57"/>
+      <c r="R22" s="57"/>
+      <c r="S22" s="57"/>
+      <c r="T22" s="57"/>
+      <c r="U22" s="57"/>
+      <c r="V22" s="57"/>
+      <c r="W22" s="57"/>
+      <c r="X22" s="57"/>
+      <c r="Y22" s="71"/>
     </row>
     <row r="23" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
@@ -3980,19 +3970,19 @@
       <c r="J23" s="8">
         <v>58.6486434937</v>
       </c>
-      <c r="K23" s="65"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="60"/>
-      <c r="P23" s="60"/>
-      <c r="Q23" s="60"/>
-      <c r="R23" s="60"/>
-      <c r="S23" s="60"/>
-      <c r="T23" s="60"/>
-      <c r="U23" s="60"/>
-      <c r="V23" s="60"/>
-      <c r="W23" s="60"/>
-      <c r="X23" s="60"/>
-      <c r="Y23" s="55"/>
+      <c r="K23" s="68"/>
+      <c r="N23" s="70"/>
+      <c r="O23" s="57"/>
+      <c r="P23" s="57"/>
+      <c r="Q23" s="57"/>
+      <c r="R23" s="57"/>
+      <c r="S23" s="57"/>
+      <c r="T23" s="57"/>
+      <c r="U23" s="57"/>
+      <c r="V23" s="57"/>
+      <c r="W23" s="57"/>
+      <c r="X23" s="57"/>
+      <c r="Y23" s="71"/>
     </row>
     <row r="24" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
@@ -4025,39 +4015,39 @@
       <c r="J24" s="6">
         <v>55.568218231199999</v>
       </c>
-      <c r="K24" s="65"/>
-      <c r="N24" s="62"/>
-      <c r="O24" s="60" t="s">
+      <c r="K24" s="68"/>
+      <c r="N24" s="70"/>
+      <c r="O24" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="P24" s="60" t="s">
+      <c r="P24" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="Q24" s="60" t="s">
+      <c r="Q24" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="R24" s="60" t="s">
+      <c r="R24" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="S24" s="60" t="s">
+      <c r="S24" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="T24" s="60" t="s">
+      <c r="T24" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="U24" s="60" t="s">
+      <c r="U24" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="V24" s="60" t="s">
+      <c r="V24" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="W24" s="60" t="s">
+      <c r="W24" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="X24" s="60" t="s">
+      <c r="X24" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="Y24" s="55"/>
+      <c r="Y24" s="71"/>
     </row>
     <row r="25" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
@@ -4090,19 +4080,19 @@
       <c r="J25" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="K25" s="65"/>
-      <c r="N25" s="62"/>
-      <c r="O25" s="60"/>
-      <c r="P25" s="60"/>
-      <c r="Q25" s="60"/>
-      <c r="R25" s="60"/>
-      <c r="S25" s="60"/>
-      <c r="T25" s="60"/>
-      <c r="U25" s="60"/>
-      <c r="V25" s="60"/>
-      <c r="W25" s="60"/>
-      <c r="X25" s="60"/>
-      <c r="Y25" s="55"/>
+      <c r="K25" s="68"/>
+      <c r="N25" s="70"/>
+      <c r="O25" s="57"/>
+      <c r="P25" s="57"/>
+      <c r="Q25" s="57"/>
+      <c r="R25" s="57"/>
+      <c r="S25" s="57"/>
+      <c r="T25" s="57"/>
+      <c r="U25" s="57"/>
+      <c r="V25" s="57"/>
+      <c r="W25" s="57"/>
+      <c r="X25" s="57"/>
+      <c r="Y25" s="71"/>
     </row>
     <row r="26" spans="1:25" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
@@ -4135,19 +4125,19 @@
       <c r="J26" s="8">
         <v>45.043037414600001</v>
       </c>
-      <c r="K26" s="65"/>
-      <c r="N26" s="62"/>
-      <c r="O26" s="60"/>
-      <c r="P26" s="60"/>
-      <c r="Q26" s="60"/>
-      <c r="R26" s="60"/>
-      <c r="S26" s="60"/>
-      <c r="T26" s="60"/>
-      <c r="U26" s="60"/>
-      <c r="V26" s="60"/>
-      <c r="W26" s="60"/>
-      <c r="X26" s="60"/>
-      <c r="Y26" s="55"/>
+      <c r="K26" s="68"/>
+      <c r="N26" s="70"/>
+      <c r="O26" s="57"/>
+      <c r="P26" s="57"/>
+      <c r="Q26" s="57"/>
+      <c r="R26" s="57"/>
+      <c r="S26" s="57"/>
+      <c r="T26" s="57"/>
+      <c r="U26" s="57"/>
+      <c r="V26" s="57"/>
+      <c r="W26" s="57"/>
+      <c r="X26" s="57"/>
+      <c r="Y26" s="71"/>
     </row>
     <row r="27" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
@@ -4181,34 +4171,34 @@
         <v>42.910861969000003</v>
       </c>
       <c r="K27" s="2"/>
-      <c r="O27" s="60" t="s">
+      <c r="O27" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="P27" s="60" t="s">
+      <c r="P27" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="Q27" s="60" t="s">
+      <c r="Q27" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="R27" s="60" t="s">
+      <c r="R27" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="S27" s="60" t="s">
+      <c r="S27" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="T27" s="60" t="s">
+      <c r="T27" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="U27" s="60" t="s">
+      <c r="U27" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="V27" s="60" t="s">
+      <c r="V27" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="W27" s="60" t="s">
+      <c r="W27" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="X27" s="60" t="s">
+      <c r="X27" s="57" t="s">
         <v>93</v>
       </c>
     </row>
@@ -4244,16 +4234,16 @@
         <v>102</v>
       </c>
       <c r="K28" s="2"/>
-      <c r="O28" s="60"/>
-      <c r="P28" s="60"/>
-      <c r="Q28" s="60"/>
-      <c r="R28" s="60"/>
-      <c r="S28" s="60"/>
-      <c r="T28" s="60"/>
-      <c r="U28" s="60"/>
-      <c r="V28" s="60"/>
-      <c r="W28" s="60"/>
-      <c r="X28" s="60"/>
+      <c r="O28" s="57"/>
+      <c r="P28" s="57"/>
+      <c r="Q28" s="57"/>
+      <c r="R28" s="57"/>
+      <c r="S28" s="57"/>
+      <c r="T28" s="57"/>
+      <c r="U28" s="57"/>
+      <c r="V28" s="57"/>
+      <c r="W28" s="57"/>
+      <c r="X28" s="57"/>
     </row>
     <row r="29" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
@@ -4287,16 +4277,16 @@
         <v>29.5980644226</v>
       </c>
       <c r="K29" s="2"/>
-      <c r="O29" s="60"/>
-      <c r="P29" s="60"/>
-      <c r="Q29" s="60"/>
-      <c r="R29" s="60"/>
-      <c r="S29" s="60"/>
-      <c r="T29" s="60"/>
-      <c r="U29" s="60"/>
-      <c r="V29" s="60"/>
-      <c r="W29" s="60"/>
-      <c r="X29" s="60"/>
+      <c r="O29" s="57"/>
+      <c r="P29" s="57"/>
+      <c r="Q29" s="57"/>
+      <c r="R29" s="57"/>
+      <c r="S29" s="57"/>
+      <c r="T29" s="57"/>
+      <c r="U29" s="57"/>
+      <c r="V29" s="57"/>
+      <c r="W29" s="57"/>
+      <c r="X29" s="57"/>
     </row>
     <row r="30" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
@@ -4327,28 +4317,28 @@
       <c r="J30" s="5"/>
       <c r="K30" s="2"/>
       <c r="O30" s="42"/>
-      <c r="P30" s="66" t="s">
+      <c r="P30" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="Q30" s="60" t="s">
+      <c r="Q30" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="R30" s="60" t="s">
+      <c r="R30" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="S30" s="60" t="s">
+      <c r="S30" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="T30" s="60" t="s">
+      <c r="T30" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="U30" s="60" t="s">
+      <c r="U30" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="V30" s="60" t="s">
+      <c r="V30" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="W30" s="69" t="s">
+      <c r="W30" s="63" t="s">
         <v>101</v>
       </c>
       <c r="X30" s="42"/>
@@ -4382,14 +4372,14 @@
       <c r="J31" s="5"/>
       <c r="K31" s="17"/>
       <c r="O31" s="42"/>
-      <c r="P31" s="67"/>
-      <c r="Q31" s="60"/>
-      <c r="R31" s="60"/>
-      <c r="S31" s="60"/>
-      <c r="T31" s="60"/>
-      <c r="U31" s="60"/>
-      <c r="V31" s="60"/>
-      <c r="W31" s="70"/>
+      <c r="P31" s="59"/>
+      <c r="Q31" s="57"/>
+      <c r="R31" s="57"/>
+      <c r="S31" s="57"/>
+      <c r="T31" s="57"/>
+      <c r="U31" s="57"/>
+      <c r="V31" s="57"/>
+      <c r="W31" s="64"/>
       <c r="X31" s="42"/>
     </row>
     <row r="32" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4421,14 +4411,14 @@
       <c r="J32" s="5"/>
       <c r="K32" s="17"/>
       <c r="O32" s="42"/>
-      <c r="P32" s="68"/>
-      <c r="Q32" s="60"/>
-      <c r="R32" s="60"/>
-      <c r="S32" s="60"/>
-      <c r="T32" s="60"/>
-      <c r="U32" s="60"/>
-      <c r="V32" s="60"/>
-      <c r="W32" s="71"/>
+      <c r="P32" s="60"/>
+      <c r="Q32" s="57"/>
+      <c r="R32" s="57"/>
+      <c r="S32" s="57"/>
+      <c r="T32" s="57"/>
+      <c r="U32" s="57"/>
+      <c r="V32" s="57"/>
+      <c r="W32" s="65"/>
       <c r="X32" s="42"/>
     </row>
     <row r="33" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4455,28 +4445,28 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="2"/>
-      <c r="O33" s="56"/>
+      <c r="O33" s="72"/>
       <c r="P33" s="42"/>
-      <c r="Q33" s="60" t="s">
+      <c r="Q33" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="R33" s="60" t="s">
+      <c r="R33" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="S33" s="60" t="s">
+      <c r="S33" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="T33" s="60" t="s">
+      <c r="T33" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="U33" s="60" t="s">
+      <c r="U33" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="V33" s="60" t="s">
+      <c r="V33" s="57" t="s">
         <v>107</v>
       </c>
       <c r="W33" s="42"/>
-      <c r="X33" s="57"/>
+      <c r="X33" s="73"/>
     </row>
     <row r="34" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
@@ -4502,16 +4492,16 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="2"/>
-      <c r="O34" s="56"/>
+      <c r="O34" s="72"/>
       <c r="P34" s="42"/>
-      <c r="Q34" s="60"/>
-      <c r="R34" s="60"/>
-      <c r="S34" s="60"/>
-      <c r="T34" s="60"/>
-      <c r="U34" s="60"/>
-      <c r="V34" s="60"/>
+      <c r="Q34" s="57"/>
+      <c r="R34" s="57"/>
+      <c r="S34" s="57"/>
+      <c r="T34" s="57"/>
+      <c r="U34" s="57"/>
+      <c r="V34" s="57"/>
       <c r="W34" s="42"/>
-      <c r="X34" s="57"/>
+      <c r="X34" s="73"/>
     </row>
     <row r="35" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
@@ -4537,16 +4527,16 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="2"/>
-      <c r="O35" s="56"/>
+      <c r="O35" s="72"/>
       <c r="P35" s="42"/>
-      <c r="Q35" s="60"/>
-      <c r="R35" s="60"/>
-      <c r="S35" s="60"/>
-      <c r="T35" s="60"/>
-      <c r="U35" s="60"/>
-      <c r="V35" s="60"/>
+      <c r="Q35" s="57"/>
+      <c r="R35" s="57"/>
+      <c r="S35" s="57"/>
+      <c r="T35" s="57"/>
+      <c r="U35" s="57"/>
+      <c r="V35" s="57"/>
       <c r="W35" s="42"/>
-      <c r="X35" s="57"/>
+      <c r="X35" s="73"/>
     </row>
     <row r="36" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A36" s="11"/>
@@ -4560,10 +4550,10 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-      <c r="R36" s="58"/>
-      <c r="S36" s="58"/>
-      <c r="T36" s="58"/>
-      <c r="U36" s="58"/>
+      <c r="R36" s="74"/>
+      <c r="S36" s="74"/>
+      <c r="T36" s="74"/>
+      <c r="U36" s="74"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
@@ -4577,12 +4567,12 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-      <c r="R37" s="59" t="s">
+      <c r="R37" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="S37" s="59"/>
-      <c r="T37" s="59"/>
-      <c r="U37" s="59"/>
+      <c r="S37" s="75"/>
+      <c r="T37" s="75"/>
+      <c r="U37" s="75"/>
     </row>
     <row r="38" spans="1:24" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="str">
@@ -4601,10 +4591,10 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
-      <c r="R38" s="59"/>
-      <c r="S38" s="59"/>
-      <c r="T38" s="59"/>
-      <c r="U38" s="59"/>
+      <c r="R38" s="75"/>
+      <c r="S38" s="75"/>
+      <c r="T38" s="75"/>
+      <c r="U38" s="75"/>
     </row>
     <row r="39" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
@@ -4635,7 +4625,7 @@
       </c>
       <c r="B40" s="26" t="str">
         <f ca="1">ROUNDUP(I140,2)&amp;"%"</f>
-        <v>72,73%</v>
+        <v>72.73%</v>
       </c>
       <c r="C40" s="29">
         <f ca="1">ROUNDUP(STDEVA(G52:G139),1)</f>
@@ -4665,7 +4655,7 @@
       </c>
       <c r="B41" s="27" t="str">
         <f ca="1">ROUNDUP(J140,2)&amp;"%"</f>
-        <v>57,96%</v>
+        <v>57.96%</v>
       </c>
       <c r="C41" s="30"/>
       <c r="D41" s="2"/>
@@ -4699,13 +4689,13 @@
       <c r="O42" s="20"/>
     </row>
     <row r="43" spans="1:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="63"/>
-      <c r="B43" s="64"/>
-      <c r="C43" s="64"/>
-      <c r="D43" s="64"/>
-      <c r="E43" s="64"/>
-      <c r="F43" s="64"/>
-      <c r="G43" s="64"/>
+      <c r="A43" s="66"/>
+      <c r="B43" s="67"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="67"/>
       <c r="H43" s="17"/>
       <c r="I43" s="17"/>
       <c r="J43" s="2"/>
@@ -4770,7 +4760,7 @@
       <c r="C48" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="D48" s="75"/>
+      <c r="D48" s="55"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -5168,7 +5158,7 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B63" s="19">
         <f>AVERAGE($F$52:$F$139)</f>
@@ -5204,7 +5194,7 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B64" s="19">
         <f ca="1">AVERAGE($G$52:$G$139)</f>
@@ -7447,41 +7437,55 @@
     </row>
   </sheetData>
   <mergeCells count="100">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="Q6:Q8"/>
-    <mergeCell ref="R6:R8"/>
-    <mergeCell ref="S6:S8"/>
-    <mergeCell ref="P9:P11"/>
-    <mergeCell ref="Q9:Q11"/>
-    <mergeCell ref="R9:R11"/>
-    <mergeCell ref="S9:S11"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="O6:O8"/>
-    <mergeCell ref="T6:T8"/>
-    <mergeCell ref="U6:U8"/>
-    <mergeCell ref="W9:W11"/>
-    <mergeCell ref="O12:O14"/>
-    <mergeCell ref="P12:P14"/>
-    <mergeCell ref="Q12:Q14"/>
-    <mergeCell ref="R12:R14"/>
-    <mergeCell ref="S12:S14"/>
-    <mergeCell ref="W12:W14"/>
-    <mergeCell ref="V12:V14"/>
-    <mergeCell ref="W18:W20"/>
-    <mergeCell ref="X12:X14"/>
-    <mergeCell ref="O15:O17"/>
-    <mergeCell ref="P15:P17"/>
-    <mergeCell ref="Q15:Q17"/>
-    <mergeCell ref="R15:R17"/>
-    <mergeCell ref="S15:S17"/>
-    <mergeCell ref="W15:W17"/>
-    <mergeCell ref="X15:X17"/>
-    <mergeCell ref="T12:T14"/>
-    <mergeCell ref="U12:U14"/>
-    <mergeCell ref="T15:T17"/>
-    <mergeCell ref="U15:U17"/>
-    <mergeCell ref="V15:V17"/>
-    <mergeCell ref="T18:T20"/>
+    <mergeCell ref="Y15:Y26"/>
+    <mergeCell ref="O33:O35"/>
+    <mergeCell ref="X33:X35"/>
+    <mergeCell ref="R36:U36"/>
+    <mergeCell ref="R37:U38"/>
+    <mergeCell ref="Q33:Q35"/>
+    <mergeCell ref="R33:R35"/>
+    <mergeCell ref="S33:S35"/>
+    <mergeCell ref="T24:T26"/>
+    <mergeCell ref="U24:U26"/>
+    <mergeCell ref="V24:V26"/>
+    <mergeCell ref="W27:W29"/>
+    <mergeCell ref="X27:X29"/>
+    <mergeCell ref="W24:W26"/>
+    <mergeCell ref="X24:X26"/>
+    <mergeCell ref="T27:T29"/>
+    <mergeCell ref="X6:X8"/>
+    <mergeCell ref="N15:N26"/>
+    <mergeCell ref="O27:O29"/>
+    <mergeCell ref="P27:P29"/>
+    <mergeCell ref="Q27:Q29"/>
+    <mergeCell ref="R27:R29"/>
+    <mergeCell ref="S27:S29"/>
+    <mergeCell ref="O24:O26"/>
+    <mergeCell ref="P24:P26"/>
+    <mergeCell ref="Q24:Q26"/>
+    <mergeCell ref="R24:R26"/>
+    <mergeCell ref="S24:S26"/>
+    <mergeCell ref="W21:W23"/>
+    <mergeCell ref="X21:X23"/>
+    <mergeCell ref="O21:O23"/>
+    <mergeCell ref="P21:P23"/>
+    <mergeCell ref="Q21:Q23"/>
+    <mergeCell ref="R21:R23"/>
+    <mergeCell ref="S21:S23"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="V18:V20"/>
+    <mergeCell ref="S18:S20"/>
+    <mergeCell ref="V6:V8"/>
+    <mergeCell ref="T9:T11"/>
+    <mergeCell ref="U9:U11"/>
+    <mergeCell ref="V9:V11"/>
+    <mergeCell ref="T33:T35"/>
+    <mergeCell ref="U33:U35"/>
+    <mergeCell ref="V33:V35"/>
+    <mergeCell ref="T21:T23"/>
+    <mergeCell ref="U21:U23"/>
+    <mergeCell ref="U27:U29"/>
+    <mergeCell ref="V27:V29"/>
     <mergeCell ref="A43:G43"/>
     <mergeCell ref="K15:K26"/>
     <mergeCell ref="X18:X20"/>
@@ -7498,55 +7502,41 @@
     <mergeCell ref="P18:P20"/>
     <mergeCell ref="Q18:Q20"/>
     <mergeCell ref="R18:R20"/>
-    <mergeCell ref="V6:V8"/>
-    <mergeCell ref="T9:T11"/>
-    <mergeCell ref="U9:U11"/>
-    <mergeCell ref="V9:V11"/>
-    <mergeCell ref="T33:T35"/>
-    <mergeCell ref="U33:U35"/>
-    <mergeCell ref="V33:V35"/>
-    <mergeCell ref="T21:T23"/>
-    <mergeCell ref="U21:U23"/>
-    <mergeCell ref="U27:U29"/>
-    <mergeCell ref="V27:V29"/>
-    <mergeCell ref="Q21:Q23"/>
-    <mergeCell ref="R21:R23"/>
-    <mergeCell ref="S21:S23"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="V18:V20"/>
-    <mergeCell ref="S18:S20"/>
-    <mergeCell ref="X6:X8"/>
-    <mergeCell ref="N15:N26"/>
-    <mergeCell ref="O27:O29"/>
-    <mergeCell ref="P27:P29"/>
-    <mergeCell ref="Q27:Q29"/>
-    <mergeCell ref="R27:R29"/>
-    <mergeCell ref="S27:S29"/>
-    <mergeCell ref="O24:O26"/>
-    <mergeCell ref="P24:P26"/>
-    <mergeCell ref="Q24:Q26"/>
-    <mergeCell ref="R24:R26"/>
-    <mergeCell ref="S24:S26"/>
-    <mergeCell ref="W21:W23"/>
-    <mergeCell ref="X21:X23"/>
-    <mergeCell ref="O21:O23"/>
-    <mergeCell ref="P21:P23"/>
-    <mergeCell ref="Y15:Y26"/>
-    <mergeCell ref="O33:O35"/>
-    <mergeCell ref="X33:X35"/>
-    <mergeCell ref="R36:U36"/>
-    <mergeCell ref="R37:U38"/>
-    <mergeCell ref="Q33:Q35"/>
-    <mergeCell ref="R33:R35"/>
-    <mergeCell ref="S33:S35"/>
-    <mergeCell ref="T24:T26"/>
-    <mergeCell ref="U24:U26"/>
-    <mergeCell ref="V24:V26"/>
-    <mergeCell ref="W27:W29"/>
-    <mergeCell ref="X27:X29"/>
-    <mergeCell ref="W24:W26"/>
-    <mergeCell ref="X24:X26"/>
-    <mergeCell ref="T27:T29"/>
+    <mergeCell ref="W18:W20"/>
+    <mergeCell ref="X12:X14"/>
+    <mergeCell ref="O15:O17"/>
+    <mergeCell ref="P15:P17"/>
+    <mergeCell ref="Q15:Q17"/>
+    <mergeCell ref="R15:R17"/>
+    <mergeCell ref="S15:S17"/>
+    <mergeCell ref="W15:W17"/>
+    <mergeCell ref="X15:X17"/>
+    <mergeCell ref="T12:T14"/>
+    <mergeCell ref="U12:U14"/>
+    <mergeCell ref="T15:T17"/>
+    <mergeCell ref="U15:U17"/>
+    <mergeCell ref="V15:V17"/>
+    <mergeCell ref="T18:T20"/>
+    <mergeCell ref="W9:W11"/>
+    <mergeCell ref="O12:O14"/>
+    <mergeCell ref="P12:P14"/>
+    <mergeCell ref="Q12:Q14"/>
+    <mergeCell ref="R12:R14"/>
+    <mergeCell ref="S12:S14"/>
+    <mergeCell ref="W12:W14"/>
+    <mergeCell ref="V12:V14"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="Q6:Q8"/>
+    <mergeCell ref="R6:R8"/>
+    <mergeCell ref="S6:S8"/>
+    <mergeCell ref="P9:P11"/>
+    <mergeCell ref="Q9:Q11"/>
+    <mergeCell ref="R9:R11"/>
+    <mergeCell ref="S9:S11"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="O6:O8"/>
+    <mergeCell ref="T6:T8"/>
+    <mergeCell ref="U6:U8"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="B32:I32 C6:H6 B9:I9 A12:J12 A15:J15 A18:J18 A21:J21 A24:J24 A27:J27 B30:I30 C33:H33">

</xml_diff>